<commit_message>
Corrigir problema com os botões Edit e Delete
</commit_message>
<xml_diff>
--- a/todo_list.xlsx
+++ b/todo_list.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,19 +740,35 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>teste</t>
+          <t>testeeeeeee</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>2024-01-26 17:00:39</t>
-        </is>
-      </c>
-    </row>
+          <t>2024-01-26 17:33:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>24</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Oiiiiiiiii</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2024-01-26 17:43:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="24"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>